<commit_message>
MNT: solve git confusion happened during rebase
</commit_message>
<xml_diff>
--- a/xpdacq/tests/999999_sample.xlsx
+++ b/xpdacq/tests/999999_sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="990"/>
+    <workbookView xWindow="2500" yWindow="3020" windowWidth="25600" windowHeight="15460" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -749,7 +749,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>